<commit_message>
AddEmployeePage testScript run. Excel Data Updated(BloodGroup)
</commit_message>
<xml_diff>
--- a/com.OnlineLeaveApplication.framework.SDET37/src/test/resources/OlmEmployeeData.xlsx
+++ b/com.OnlineLeaveApplication.framework.SDET37/src/test/resources/OlmEmployeeData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91900\git\OnlineLeaveApplication\com.OnlineLeaveApplication.framework.SDET37\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHUBH\git\OnlineLeaveApplication\com.OnlineLeaveApplication.framework.SDET37\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44080AE-89F5-44B2-B143-2AB3A1C862AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86350833-AF40-4E43-AF74-208109E90DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee_Data" sheetId="1" r:id="rId1"/>
+    <sheet name="DataProviderExcel" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="146">
   <si>
     <t>Department_Name</t>
   </si>
@@ -144,9 +145,6 @@
     <t>TR</t>
   </si>
   <si>
-    <t>O+ve</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -406,6 +404,66 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>EmpName</t>
+  </si>
+  <si>
+    <t>Satish</t>
+  </si>
+  <si>
+    <t>Sanket</t>
+  </si>
+  <si>
+    <t>Shushil</t>
+  </si>
+  <si>
+    <t>EmpCode</t>
+  </si>
+  <si>
+    <t>Sa5566</t>
+  </si>
+  <si>
+    <t>Sa6655</t>
+  </si>
+  <si>
+    <t>Sh6565</t>
+  </si>
+  <si>
+    <t>Shyam</t>
+  </si>
+  <si>
+    <t>Sh5656</t>
+  </si>
+  <si>
+    <t>Sr no</t>
+  </si>
+  <si>
+    <t>O+</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>BloodGroupDropdown</t>
+  </si>
+  <si>
+    <t>AB+</t>
+  </si>
+  <si>
+    <t>AB-</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>O-</t>
   </si>
 </sst>
 </file>
@@ -447,7 +505,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,8 +524,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -490,12 +560,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -504,9 +585,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,6 +612,19 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -817,30 +908,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="24" customWidth="1"/>
-    <col min="13" max="13" width="23.33203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="29.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="24" style="3" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="29.42578125" customWidth="1"/>
     <col min="15" max="15" width="31" customWidth="1"/>
+    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="10">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="9">
         <v>0</v>
       </c>
       <c r="B1" s="1">
@@ -873,11 +966,11 @@
       <c r="K1" s="1">
         <v>10</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1" s="2">
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N1" s="1">
         <v>13</v>
@@ -885,558 +978,587 @@
       <c r="O1" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+      <c r="P1" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="F3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="6">
+        <v>35709</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="7">
+        <v>9874563201</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="O2" s="11" t="s">
+      <c r="O3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="6">
+        <v>34978</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="7">
+        <v>7418552963</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="6">
+        <v>33729</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="7">
+        <v>9635258741</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="O5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="6">
+        <v>35407</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="7">
+        <v>9874956321</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="7">
+        <v>8523869741</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="6">
+        <v>34425</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="7">
+        <v>9875244630</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="P8" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="6">
+        <v>34281</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L9" s="7">
+        <v>1236547890</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="P9" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" s="6">
+        <v>34520</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="7">
+        <v>8796541563</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="P10" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="7">
-        <v>35709</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="6">
+        <v>34822</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="5">
-        <v>9874563201</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="L11" s="7">
+        <v>9916785433</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" s="6">
+        <v>34794</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="7">
-        <v>34978</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="5">
-        <v>7418552963</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="7">
-        <v>33729</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="5">
-        <v>9635258741</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="K12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L12" s="7">
+        <v>8123654879</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" s="7">
-        <v>35407</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="5">
-        <v>9874956321</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="5">
-        <v>8523869741</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="7">
-        <v>34425</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="5">
-        <v>9875244630</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="6">
+        <v>33299</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="7">
-        <v>34281</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K9" s="5" t="s">
+      <c r="K13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="7">
+        <v>9874812356</v>
+      </c>
+      <c r="M13" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="L9" s="5">
-        <v>1236547890</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" s="7">
-        <v>34520</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="L10" s="5">
-        <v>8796541563</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I11" s="7">
-        <v>34822</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="5">
-        <v>9916785433</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I12" s="7">
-        <v>34794</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="L12" s="5">
-        <v>8123654879</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="N12" s="5" t="s">
+      <c r="N13" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="O13" s="4" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I13" s="7">
-        <v>33299</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L13" s="5">
-        <v>9874812356</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1458,4 +1580,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7357277B-BB9D-40AC-8270-07DFC9E5B89E}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>